<commit_message>
removed ALL option in supplier scope for #% of Vol, fixed logic for # of volume awarded
</commit_message>
<xml_diff>
--- a/default_data 1.xlsx
+++ b/default_data 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PHWATES\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrisw78\RFP Automation REPO\RFP_Analysis_Automation2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548C5F79-F38C-474F-8E52-8E140AC01721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6284CAB-BEB3-4C29-8F79-A1184EBF12B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="818" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28950" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="818" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item Attributes" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Capacity!$A$1:$B$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Item Attributes'!$A$1:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Price!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Supplier Bid Attributes'!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="51">
   <si>
     <t>Bid ID</t>
   </si>
@@ -867,10 +869,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,18 +899,15 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>70</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -916,10 +915,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -927,43 +926,43 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>60</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>55</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -979,35 +978,35 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11">
-        <v>23</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1015,10 +1014,10 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1034,35 +1033,35 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>24</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1078,35 +1077,35 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19">
-        <v>64</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1114,10 +1113,10 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22">
-        <v>97</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1133,35 +1132,35 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>13</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C26">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1177,49 +1176,43 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
       </c>
       <c r="C28">
-        <v>13</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31">
-        <v>75</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C31">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <customProperties>
     <customPr name="GUID" r:id="rId1"/>
@@ -1231,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E028EDA-D80C-428B-8F42-565A70750B1D}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,16 +1273,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>420</v>
+        <v>499</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
         <v>50</v>
@@ -1297,19 +1290,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>410</v>
+        <v>500</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1317,44 +1310,44 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>430</v>
+        <v>500</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>450</v>
+        <v>690</v>
       </c>
       <c r="D6" t="s">
         <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>460</v>
+        <v>590</v>
       </c>
       <c r="D7" t="s">
         <v>33</v>
@@ -1368,50 +1361,50 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>470</v>
+        <v>420</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>480</v>
+        <v>610</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>490</v>
+        <v>510</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1419,13 +1412,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C11">
-        <v>500</v>
+        <v>410</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
         <v>50</v>
@@ -1436,10 +1429,10 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C12">
-        <v>499</v>
+        <v>620</v>
       </c>
       <c r="D12" t="s">
         <v>35</v>
@@ -1450,36 +1443,36 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>610</v>
+        <v>520</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>620</v>
+        <v>430</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1501,36 +1494,36 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16">
-        <v>640</v>
+        <v>530</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>650</v>
+        <v>450</v>
       </c>
       <c r="D17" t="s">
         <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1538,10 +1531,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C18">
-        <v>660</v>
+        <v>640</v>
       </c>
       <c r="D18" t="s">
         <v>35</v>
@@ -1552,36 +1545,36 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C19">
-        <v>670</v>
+        <v>540</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>680</v>
+        <v>460</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1589,10 +1582,10 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>690</v>
+        <v>650</v>
       </c>
       <c r="D21" t="s">
         <v>35</v>
@@ -1606,10 +1599,10 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="D22" t="s">
         <v>33</v>
@@ -1620,16 +1613,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C23">
-        <v>510</v>
+        <v>470</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E23" t="s">
         <v>49</v>
@@ -1637,19 +1630,19 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>520</v>
+        <v>660</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1657,10 +1650,10 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C25">
-        <v>530</v>
+        <v>560</v>
       </c>
       <c r="D25" t="s">
         <v>33</v>
@@ -1671,16 +1664,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C26">
-        <v>540</v>
+        <v>480</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
         <v>49</v>
@@ -1688,19 +1681,19 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C27">
-        <v>550</v>
+        <v>670</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1708,13 +1701,13 @@
         <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>560</v>
+        <v>570</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
         <v>49</v>
@@ -1722,36 +1715,36 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>570</v>
+        <v>490</v>
       </c>
       <c r="D29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
       </c>
       <c r="C30">
-        <v>580</v>
+        <v>680</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1759,19 +1752,24 @@
         <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31">
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E31" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{2E028EDA-D80C-428B-8F42-565A70750B1D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E31">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <customProperties>
     <customPr name="GUID" r:id="rId1"/>

</xml_diff>